<commit_message>
All softwares updated working fine
</commit_message>
<xml_diff>
--- a/testData/SFI_AllMobile_Tbl_Live.xlsx
+++ b/testData/SFI_AllMobile_Tbl_Live.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
   <si>
     <t>BuildUrl</t>
   </si>
@@ -298,12 +298,30 @@
   </si>
   <si>
     <t>Choose the value..!</t>
+  </si>
+  <si>
+    <t>date_range
+Appointment Date : 26/12/2023, Time : [ 09:00 AM to 09:04 AM ]</t>
+  </si>
+  <si>
+    <t>26/12/2023</t>
+  </si>
+  <si>
+    <t>voice_record_26122023</t>
+  </si>
+  <si>
+    <t>formshow_26122023</t>
+  </si>
+  <si>
+    <t>date_range
+Appointment Date : 26/12/2023, Time : [ 09:05 AM to 09:09 AM ]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -643,195 +661,195 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="4" max="4" width="52.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="52.1796875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.54296875"/>
+    <col min="3" max="3" customWidth="true" width="16.54296875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="52.1796875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.90625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.54296875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="21.7265625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.7265625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.54296875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.453125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="27.7265625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.81640625"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="27.6328125"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.0"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.36328125"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="27.1796875"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="26.54296875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="14.6328125"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="16.54296875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.81640625"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.26953125"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="8.81640625"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.36328125"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="16.54296875"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.26953125"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="15.08984375"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.6328125"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="19.26953125"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="27.54296875"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="34.54296875"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="16.08984375"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="26.54296875"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="30.26953125"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="16.26953125"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="9.26953125"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="19.453125"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="21.1796875"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="28.26953125"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="20.7265625"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="13.6328125"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AO1" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS1" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AV1" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -845,19 +863,19 @@
       <c r="C2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>47</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -866,118 +884,118 @@
       <c r="J2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="0">
         <v>1234567890</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="N2" t="s">
-        <v>88</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="O2" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="0">
         <v>1234567890</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="0">
         <v>50</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="0">
         <v>9</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="AB2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AB2" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="AC2" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AI2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AJ2" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AK2" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AL2" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AM2" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AN2" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AO2" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AP2" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AQ2" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="AR2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS2" t="s">
+      <c r="AR2" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="AS2" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AT2" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="AU2" t="s">
-        <v>91</v>
+      <c r="AU2" t="s" s="0">
+        <v>96</v>
       </c>
       <c r="AV2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2" t="s" s="0">
         <v>68</v>
       </c>
     </row>

</xml_diff>